<commit_message>
ADD: Explore model for HighU-vs-HighJ-vs-Both-vs-None
</commit_message>
<xml_diff>
--- a/temporary_files/explored_highj.xlsx
+++ b/temporary_files/explored_highj.xlsx
@@ -1,95 +1,88 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edgarduron/Documents/Working-Papers/AppStore-Research/AppStore_Analysis/AppStore/temporary_files/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D735ECC-3F91-0147-84A0-EFF8938A30A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="16460" windowHeight="12920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
-    <t>term</t>
-  </si>
-  <si>
-    <t>estimate</t>
-  </si>
-  <si>
-    <t>std.error</t>
-  </si>
-  <si>
-    <t>statistic</t>
-  </si>
-  <si>
-    <t>p.value</t>
-  </si>
-  <si>
-    <t>(Intercept)</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>genderFemale</t>
-  </si>
-  <si>
-    <t>income</t>
-  </si>
-  <si>
-    <t>visit_frequency</t>
-  </si>
-  <si>
-    <t>app_expense</t>
-  </si>
-  <si>
-    <t>previous_experience</t>
-  </si>
-  <si>
-    <t>regulatory_focusPrevention</t>
-  </si>
-  <si>
-    <t>platform_preferenceAppStore</t>
-  </si>
-  <si>
-    <t>involvement1</t>
-  </si>
-  <si>
-    <t>factor(highJ_apporder)2</t>
-  </si>
-  <si>
-    <t>factor(highJ_apporder)3</t>
-  </si>
-  <si>
-    <t>factor(highJ_apporder)4</t>
-  </si>
-  <si>
-    <t>factor(highJ_appname)JogStats</t>
-  </si>
-  <si>
-    <t>factor(highJ_appname)Map My Walk</t>
-  </si>
-  <si>
-    <t>factor(highJ_appname)Running Watch</t>
+    <t xml:space="preserve">term</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estimate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">std.error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">statistic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Intercept)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">genderFemale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visit_frequency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app_expense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">previous_experience</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regulatory_focusPrevention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">platform_preferenceAppStore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">involvement1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">factor(highJ_apporder)2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">factor(highJ_apporder)3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">factor(highJ_apporder)4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">factor(highJ_appname)JogStats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">factor(highJ_appname)Map My Walk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">factor(highJ_appname)Running Watch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -125,15 +118,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -415,16 +399,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,280 +423,280 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>1.7470000000000001</v>
-      </c>
-      <c r="C2">
-        <v>0.82399999999999995</v>
-      </c>
-      <c r="D2">
-        <v>2.1190000000000002</v>
-      </c>
-      <c r="E2">
-        <v>3.4000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="n">
+        <v>1.747</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.824</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2.119</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.034</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>-5.0000000000000001E-3</v>
-      </c>
-      <c r="C3">
-        <v>1.2E-2</v>
-      </c>
-      <c r="D3">
+      <c r="B3" t="n">
+        <v>-0.005</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="D3" t="n">
         <v>-0.44</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="n">
         <v>0.66</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
-        <v>-0.48799999999999999</v>
-      </c>
-      <c r="C4">
+      <c r="B4" t="n">
+        <v>-0.488</v>
+      </c>
+      <c r="C4" t="n">
         <v>0.215</v>
       </c>
-      <c r="D4">
-        <v>-2.2679999999999998</v>
-      </c>
-      <c r="E4">
-        <v>2.3E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D4" t="n">
+        <v>-2.268</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.023</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="n">
         <v>0.03</v>
       </c>
-      <c r="C5">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="D5">
-        <v>0.45100000000000001</v>
-      </c>
-      <c r="E5">
-        <v>0.65200000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C5" t="n">
+        <v>0.066</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.451</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.652</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="n">
         <v>-0.111</v>
       </c>
-      <c r="C6">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="D6">
-        <v>-0.63300000000000001</v>
-      </c>
-      <c r="E6">
-        <v>0.52700000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C6" t="n">
+        <v>0.176</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-0.633</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.527</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
-        <v>1.2E-2</v>
-      </c>
-      <c r="C7">
-        <v>9.4E-2</v>
-      </c>
-      <c r="D7">
-        <v>0.13200000000000001</v>
-      </c>
-      <c r="E7">
-        <v>0.89500000000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.094</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.132</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.895</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8">
-        <v>-5.7000000000000002E-2</v>
-      </c>
-      <c r="C8">
-        <v>8.5999999999999993E-2</v>
-      </c>
-      <c r="D8">
-        <v>-0.66100000000000003</v>
-      </c>
-      <c r="E8">
-        <v>0.50900000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" t="n">
+        <v>-0.057</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.086</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-0.661</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.509</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9">
-        <v>-2.8000000000000001E-2</v>
-      </c>
-      <c r="C9">
-        <v>0.20899999999999999</v>
-      </c>
-      <c r="D9">
-        <v>-0.13600000000000001</v>
-      </c>
-      <c r="E9">
-        <v>0.89200000000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" t="n">
+        <v>-0.028</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.209</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-0.136</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.892</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10">
-        <v>-0.28599999999999998</v>
-      </c>
-      <c r="C10">
+      <c r="B10" t="n">
+        <v>-0.286</v>
+      </c>
+      <c r="C10" t="n">
         <v>0.214</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="n">
         <v>-1.335</v>
       </c>
-      <c r="E10">
+      <c r="E10" t="n">
         <v>0.182</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="C11">
-        <v>0.24099999999999999</v>
-      </c>
-      <c r="D11">
-        <v>0.57099999999999995</v>
-      </c>
-      <c r="E11">
-        <v>0.56799999999999995</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="n">
+        <v>0.138</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.241</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.571</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.568</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="n">
         <v>-0.193</v>
       </c>
-      <c r="C12">
-        <v>0.30399999999999999</v>
-      </c>
-      <c r="D12">
-        <v>-0.63700000000000001</v>
-      </c>
-      <c r="E12">
-        <v>0.52400000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C12" t="n">
+        <v>0.304</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-0.637</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.524</v>
+      </c>
+    </row>
+    <row r="13">
       <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="n">
         <v>-0.32</v>
       </c>
-      <c r="C13">
-        <v>0.30299999999999999</v>
-      </c>
-      <c r="D13">
-        <v>-1.0549999999999999</v>
-      </c>
-      <c r="E13">
-        <v>0.29099999999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C13" t="n">
+        <v>0.303</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-1.055</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.291</v>
+      </c>
+    </row>
+    <row r="14">
       <c r="A14" t="s">
         <v>17</v>
       </c>
-      <c r="B14">
-        <v>-0.17399999999999999</v>
-      </c>
-      <c r="C14">
-        <v>0.30499999999999999</v>
-      </c>
-      <c r="D14">
-        <v>-0.57099999999999995</v>
-      </c>
-      <c r="E14">
-        <v>0.56799999999999995</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" t="n">
+        <v>-0.174</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.305</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-0.571</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.568</v>
+      </c>
+    </row>
+    <row r="15">
       <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="B15">
-        <v>0.14599999999999999</v>
-      </c>
-      <c r="C15">
-        <v>0.30499999999999999</v>
-      </c>
-      <c r="D15">
+      <c r="B15" t="n">
+        <v>0.146</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.305</v>
+      </c>
+      <c r="D15" t="n">
         <v>0.48</v>
       </c>
-      <c r="E15">
-        <v>0.63100000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E15" t="n">
+        <v>0.631</v>
+      </c>
+    </row>
+    <row r="16">
       <c r="A16" t="s">
         <v>19</v>
       </c>
-      <c r="B16">
-        <v>0.14099999999999999</v>
-      </c>
-      <c r="C16">
+      <c r="B16" t="n">
+        <v>0.141</v>
+      </c>
+      <c r="C16" t="n">
         <v>0.309</v>
       </c>
-      <c r="D16">
-        <v>0.45500000000000002</v>
-      </c>
-      <c r="E16">
-        <v>0.64900000000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D16" t="n">
+        <v>0.455</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.649</v>
+      </c>
+    </row>
+    <row r="17">
       <c r="A17" t="s">
         <v>20</v>
       </c>
-      <c r="B17">
-        <v>8.4000000000000005E-2</v>
-      </c>
-      <c r="C17">
-        <v>0.26300000000000001</v>
-      </c>
-      <c r="D17">
-        <v>0.32100000000000001</v>
-      </c>
-      <c r="E17">
+      <c r="B17" t="n">
+        <v>0.084</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.263</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.321</v>
+      </c>
+      <c r="E17" t="n">
         <v>0.748</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ADD: Manipulation check, Promotion-based final results, exploration post-hoc.
</commit_message>
<xml_diff>
--- a/temporary_files/explored_highj.xlsx
+++ b/temporary_files/explored_highj.xlsx
@@ -428,16 +428,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>1.747</v>
+        <v>1.75</v>
       </c>
       <c r="C2" t="n">
-        <v>0.824</v>
+        <v>0.82</v>
       </c>
       <c r="D2" t="n">
-        <v>2.119</v>
+        <v>2.12</v>
       </c>
       <c r="E2" t="n">
-        <v>0.034</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="3">
@@ -445,10 +445,10 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.005</v>
+        <v>-0.01</v>
       </c>
       <c r="C3" t="n">
-        <v>0.012</v>
+        <v>0.01</v>
       </c>
       <c r="D3" t="n">
         <v>-0.44</v>
@@ -462,16 +462,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.488</v>
+        <v>-0.49</v>
       </c>
       <c r="C4" t="n">
-        <v>0.215</v>
+        <v>0.22</v>
       </c>
       <c r="D4" t="n">
-        <v>-2.268</v>
+        <v>-2.27</v>
       </c>
       <c r="E4" t="n">
-        <v>0.023</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="5">
@@ -482,13 +482,13 @@
         <v>0.03</v>
       </c>
       <c r="C5" t="n">
-        <v>0.066</v>
+        <v>0.07</v>
       </c>
       <c r="D5" t="n">
-        <v>0.451</v>
+        <v>0.45</v>
       </c>
       <c r="E5" t="n">
-        <v>0.652</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="6">
@@ -496,16 +496,16 @@
         <v>9</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.111</v>
+        <v>-0.11</v>
       </c>
       <c r="C6" t="n">
-        <v>0.176</v>
+        <v>0.18</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.633</v>
+        <v>-0.63</v>
       </c>
       <c r="E6" t="n">
-        <v>0.527</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="7">
@@ -513,16 +513,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>0.012</v>
+        <v>0.01</v>
       </c>
       <c r="C7" t="n">
-        <v>0.094</v>
+        <v>0.09</v>
       </c>
       <c r="D7" t="n">
-        <v>0.132</v>
+        <v>0.13</v>
       </c>
       <c r="E7" t="n">
-        <v>0.895</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="8">
@@ -530,16 +530,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.057</v>
+        <v>-0.06</v>
       </c>
       <c r="C8" t="n">
-        <v>0.086</v>
+        <v>0.09</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.661</v>
+        <v>-0.66</v>
       </c>
       <c r="E8" t="n">
-        <v>0.509</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="9">
@@ -547,16 +547,16 @@
         <v>12</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.028</v>
+        <v>-0.03</v>
       </c>
       <c r="C9" t="n">
-        <v>0.209</v>
+        <v>0.21</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.136</v>
+        <v>-0.14</v>
       </c>
       <c r="E9" t="n">
-        <v>0.892</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="10">
@@ -564,16 +564,16 @@
         <v>13</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.286</v>
+        <v>-0.29</v>
       </c>
       <c r="C10" t="n">
-        <v>0.214</v>
+        <v>0.21</v>
       </c>
       <c r="D10" t="n">
-        <v>-1.335</v>
+        <v>-1.33</v>
       </c>
       <c r="E10" t="n">
-        <v>0.182</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="11">
@@ -581,16 +581,16 @@
         <v>14</v>
       </c>
       <c r="B11" t="n">
-        <v>0.138</v>
+        <v>0.14</v>
       </c>
       <c r="C11" t="n">
-        <v>0.241</v>
+        <v>0.24</v>
       </c>
       <c r="D11" t="n">
-        <v>0.571</v>
+        <v>0.57</v>
       </c>
       <c r="E11" t="n">
-        <v>0.568</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="12">
@@ -598,16 +598,16 @@
         <v>15</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.193</v>
+        <v>-0.19</v>
       </c>
       <c r="C12" t="n">
-        <v>0.304</v>
+        <v>0.3</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.637</v>
+        <v>-0.64</v>
       </c>
       <c r="E12" t="n">
-        <v>0.524</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="13">
@@ -618,13 +618,13 @@
         <v>-0.32</v>
       </c>
       <c r="C13" t="n">
-        <v>0.303</v>
+        <v>0.3</v>
       </c>
       <c r="D13" t="n">
-        <v>-1.055</v>
+        <v>-1.06</v>
       </c>
       <c r="E13" t="n">
-        <v>0.291</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="14">
@@ -632,16 +632,16 @@
         <v>17</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.174</v>
+        <v>-0.17</v>
       </c>
       <c r="C14" t="n">
-        <v>0.305</v>
+        <v>0.3</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.571</v>
+        <v>-0.57</v>
       </c>
       <c r="E14" t="n">
-        <v>0.568</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="15">
@@ -649,16 +649,16 @@
         <v>18</v>
       </c>
       <c r="B15" t="n">
-        <v>0.146</v>
+        <v>0.15</v>
       </c>
       <c r="C15" t="n">
-        <v>0.305</v>
+        <v>0.3</v>
       </c>
       <c r="D15" t="n">
         <v>0.48</v>
       </c>
       <c r="E15" t="n">
-        <v>0.631</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="16">
@@ -666,16 +666,16 @@
         <v>19</v>
       </c>
       <c r="B16" t="n">
-        <v>0.141</v>
+        <v>0.14</v>
       </c>
       <c r="C16" t="n">
-        <v>0.309</v>
+        <v>0.31</v>
       </c>
       <c r="D16" t="n">
-        <v>0.455</v>
+        <v>0.46</v>
       </c>
       <c r="E16" t="n">
-        <v>0.649</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="17">
@@ -683,16 +683,16 @@
         <v>20</v>
       </c>
       <c r="B17" t="n">
-        <v>0.084</v>
+        <v>0.08</v>
       </c>
       <c r="C17" t="n">
-        <v>0.263</v>
+        <v>0.26</v>
       </c>
       <c r="D17" t="n">
-        <v>0.321</v>
+        <v>0.32</v>
       </c>
       <c r="E17" t="n">
-        <v>0.748</v>
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>